<commit_message>
redo: revert diarrhea inci; reduce MMN cost; rename MMN to Antenatal-; remove Zinc; add IYCF education
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="32620" windowHeight="20560" tabRatio="500" firstSheet="18" activeTab="19"/>
+    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="32620" windowHeight="20560" tabRatio="500" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     <author>Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +207,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="81">
   <si>
     <t>indicators</t>
   </si>
@@ -431,9 +453,6 @@
     <t>Vitamin A supplementation</t>
   </si>
   <si>
-    <t>Multiple micronutrient supplementation</t>
-  </si>
-  <si>
     <t>Outcome</t>
   </si>
   <si>
@@ -470,15 +489,23 @@
     <t>Public provision of complementary foods</t>
   </si>
   <si>
+    <t>Balanced energy-protein supplementation</t>
+  </si>
+  <si>
     <t>Food security &amp; education</t>
+  </si>
+  <si>
+    <t>Antenatal micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>IYCF education</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -598,7 +625,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -640,7 +667,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -649,13 +675,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1822,7 +1842,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="13">
         <v>0.56799999999999995</v>
@@ -1830,17 +1850,17 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="25">
+        <v>70</v>
+      </c>
+      <c r="B6" s="23">
         <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="25">
+        <v>72</v>
+      </c>
+      <c r="B7" s="23">
         <v>0.20599999999999999</v>
       </c>
     </row>
@@ -2477,7 +2497,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E5"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3055,7 +3075,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -3107,7 +3127,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3223,8 +3245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3255,7 +3277,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="17">
         <v>5.16</v>
@@ -3269,17 +3291,29 @@
       <c r="E2" s="18">
         <v>1.82</v>
       </c>
-      <c r="F2" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F2" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="17">
+        <v>5.16</v>
+      </c>
+      <c r="C3" s="17">
+        <v>5.16</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1.82</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1.82</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
@@ -3499,8 +3533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3527,36 +3561,36 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="19">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.621</v>
       </c>
       <c r="C2" s="6">
         <v>0.85</v>
       </c>
       <c r="D2" s="6">
-        <v>7.08</v>
+        <v>0.35</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="21"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B3" s="6">
-        <v>0.621</v>
+        <v>0.247</v>
       </c>
       <c r="C3" s="6">
         <v>0.85</v>
       </c>
       <c r="D3" s="6">
-        <v>0.35</v>
+        <v>3.56</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3564,55 +3598,55 @@
         <v>76</v>
       </c>
       <c r="B4" s="6">
-        <v>0.247</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
         <v>0.85</v>
       </c>
       <c r="D4" s="6">
-        <v>3.56</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="21"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C5" s="6">
         <v>0.85</v>
       </c>
       <c r="D5" s="6">
-        <v>48</v>
+        <v>3.56</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
-        <v>75</v>
+      <c r="A6" t="s">
+        <v>77</v>
       </c>
       <c r="B6" s="6">
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6">
         <v>0.85</v>
       </c>
       <c r="D6" s="6">
-        <v>3.56</v>
+        <v>25</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14" t="s">
-        <v>65</v>
+      <c r="A7" t="s">
+        <v>79</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -3624,12 +3658,22 @@
         <v>1.8</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3.56</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -3734,7 +3778,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3767,14 +3811,14 @@
         <v>15</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -3783,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -3797,7 +3841,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3812,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -3829,10 +3873,12 @@
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <v>1</v>
+        <f>demographics!$B$6</f>
+        <v>0.4</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <f>demographics!$B$6</f>
+        <v>0.4</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -3843,55 +3889,54 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <f>demographics!$B$6</f>
         <v>0.4</v>
       </c>
-      <c r="E5" s="4">
-        <f>demographics!$B$6</f>
-        <v>0.4</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14" t="s">
-        <v>65</v>
+      <c r="A7" t="s">
+        <v>79</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3913,11 +3958,27 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="6"/>
@@ -4018,10 +4079,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4034,7 +4095,7 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -4051,38 +4112,77 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="D2" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="E2" s="22">
-        <v>0</v>
-      </c>
-      <c r="F2" s="22">
+        <v>66</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="22">
-        <v>1</v>
-      </c>
-      <c r="D3" s="22">
-        <v>1</v>
-      </c>
-      <c r="E3" s="22">
-        <v>0</v>
-      </c>
-      <c r="F3" s="22">
+        <v>69</v>
+      </c>
+      <c r="C3" s="21">
+        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <v>0.22719999999999999</v>
+      </c>
+      <c r="D3" s="21">
+        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <v>0.22719999999999999</v>
+      </c>
+      <c r="E3" s="21">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
         <v>0</v>
       </c>
     </row>
@@ -4093,10 +4193,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4106,7 +4206,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4129,7 +4229,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4141,17 +4241,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G2" s="23">
-        <v>0.29699999999999999</v>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F2" s="22">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G2" s="22">
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -4164,55 +4263,23 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="23">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G3" s="23">
-        <v>0.29699999999999999</v>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="6"/>
@@ -4220,20 +4287,9 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4242,10 +4298,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4255,7 +4311,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4278,7 +4334,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4290,17 +4346,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F2" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G2" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -4314,54 +4369,22 @@
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>0.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.3</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="6"/>
@@ -4369,20 +4392,9 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4391,10 +4403,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4404,7 +4416,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4427,7 +4439,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4439,17 +4451,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="F2" s="6">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="G2" s="6">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -4463,54 +4474,22 @@
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>0.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.62</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="6"/>
@@ -4518,20 +4497,9 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5285,7 +5253,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5314,19 +5282,19 @@
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="23">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>2.4300000000000002</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="23">
         <v>3.71</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="23">
         <v>3</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="23">
         <v>1.92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
redefine breastfeeding promotion target and effect
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="32620" windowHeight="20560" tabRatio="500" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14240" tabRatio="500" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1472,6 +1472,108 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3245,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3286,10 +3388,10 @@
         <v>5.16</v>
       </c>
       <c r="D2" s="17">
-        <v>1.82</v>
+        <v>1</v>
       </c>
       <c r="E2" s="18">
-        <v>1.82</v>
+        <v>1</v>
       </c>
       <c r="F2" s="19">
         <v>1</v>
@@ -3332,7 +3434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3534,7 +3636,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3778,7 +3880,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3898,10 +4000,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
complementary feeding now includes effect on breastfeeding practices 6-23 months
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14240" tabRatio="500" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14240" tabRatio="500" firstSheet="17" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="81">
   <si>
     <t>indicators</t>
   </si>
@@ -1574,6 +1574,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3345,10 +3396,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3397,15 +3448,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B3" s="17">
-        <v>5.16</v>
+        <v>1</v>
       </c>
       <c r="C3" s="17">
-        <v>5.16</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17">
         <v>1.82</v>
@@ -3417,13 +3468,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="17">
+        <v>5.16</v>
+      </c>
+      <c r="C4" s="17">
+        <v>5.16</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1.82</v>
+      </c>
+      <c r="E4" s="19">
+        <v>1.82</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3434,7 +3505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3636,7 +3707,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4297,8 +4368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
remove IYCF; add pregnant women to target pop of BF promotion
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14240" tabRatio="500" firstSheet="17" activeTab="22"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14140" tabRatio="500" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="80">
   <si>
     <t>indicators</t>
   </si>
@@ -496,9 +496,6 @@
   </si>
   <si>
     <t>Antenatal micronutrient supplementation</t>
-  </si>
-  <si>
-    <t>IYCF education</t>
   </si>
 </sst>
 </file>
@@ -1625,6 +1622,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3101,7 +3149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -3396,10 +3446,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3468,33 +3518,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="17">
-        <v>5.16</v>
-      </c>
-      <c r="C4" s="17">
-        <v>5.16</v>
-      </c>
-      <c r="D4" s="17">
-        <v>1.82</v>
-      </c>
-      <c r="E4" s="19">
-        <v>1.82</v>
-      </c>
-      <c r="F4" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3704,10 +3734,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3835,18 +3865,8 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3.56</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -3888,10 +3908,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="6"/>
@@ -3936,10 +3953,6 @@
     <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3948,10 +3961,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4080,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4131,27 +4144,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="6"/>
@@ -4190,10 +4187,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="6"/>
@@ -4238,10 +4232,6 @@
     <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4368,7 +4358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -4474,7 +4464,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>